<commit_message>
Scatter plot pour la désagrégation spatiale avec agg_matrix2
Une fois fixer, la mettre dans agg_matrix, recalibrer
</commit_message>
<xml_diff>
--- a/data/agg_matrix.xlsx
+++ b/data/agg_matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -98,25 +98,13 @@
     <t xml:space="preserve">Europe</t>
   </si>
   <si>
-    <t xml:space="preserve">BRIS</t>
+    <t xml:space="preserve">BRICS</t>
   </si>
   <si>
     <t xml:space="preserve">Other_OECD</t>
   </si>
   <si>
     <t xml:space="preserve">RoW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suisse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UK</t>
   </si>
   <si>
     <t xml:space="preserve">Austria</t>
@@ -296,6 +284,9 @@
     <t xml:space="preserve">JP</t>
   </si>
   <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
     <t xml:space="preserve">CN</t>
   </si>
   <si>
@@ -415,7 +406,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -462,14 +453,6 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -603,7 +586,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -714,10 +697,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1724,7 +1703,7 @@
   </sheetPr>
   <dimension ref="A1:T201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -1732,7 +1711,7 @@
       <selection pane="bottomRight" activeCell="T201" activeCellId="0" sqref="T201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -14223,17 +14202,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="F33" activeCellId="0" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.21"/>
@@ -14241,6 +14220,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="955" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14265,25 +14245,13 @@
       <c r="G1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -14298,27 +14266,15 @@
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -14333,27 +14289,15 @@
         <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="27" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -14368,27 +14312,15 @@
         <v>0</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -14403,27 +14335,15 @@
         <v>0</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -14438,27 +14358,15 @@
         <v>0</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -14473,27 +14381,15 @@
         <v>0</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -14508,27 +14404,15 @@
         <v>0</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -14543,27 +14427,15 @@
         <v>0</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -14578,27 +14450,15 @@
         <v>0</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -14613,24 +14473,12 @@
         <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>22</v>
@@ -14650,25 +14498,13 @@
       <c r="G12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -14683,27 +14519,15 @@
         <v>0</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -14718,27 +14542,15 @@
         <v>0</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -14753,27 +14565,15 @@
         <v>0</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -14788,27 +14588,15 @@
         <v>0</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -14823,27 +14611,15 @@
         <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -14858,27 +14634,15 @@
         <v>0</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -14893,27 +14657,15 @@
         <v>0</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -14928,27 +14680,15 @@
         <v>0</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -14963,27 +14703,15 @@
         <v>0</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="27" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>0</v>
@@ -14998,27 +14726,15 @@
         <v>0</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>0</v>
@@ -15033,27 +14749,15 @@
         <v>0</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0</v>
@@ -15068,27 +14772,15 @@
         <v>0</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>0</v>
@@ -15103,27 +14795,15 @@
         <v>0</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>0</v>
@@ -15138,27 +14818,15 @@
         <v>0</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>0</v>
@@ -15173,27 +14841,15 @@
         <v>0</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>0</v>
@@ -15208,27 +14864,15 @@
         <v>0</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>0</v>
@@ -15240,30 +14884,18 @@
         <v>0</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0</v>
@@ -15275,30 +14907,18 @@
         <v>0</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>0</v>
@@ -15310,30 +14930,18 @@
         <v>0</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="27" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0</v>
@@ -15342,33 +14950,21 @@
         <v>0</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0</v>
@@ -15383,27 +14979,15 @@
         <v>1</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
@@ -15418,27 +15002,15 @@
         <v>1</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0</v>
@@ -15453,27 +15025,15 @@
         <v>0</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>0</v>
@@ -15488,27 +15048,15 @@
         <v>0</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>0</v>
@@ -15523,27 +15071,15 @@
         <v>1</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>0</v>
@@ -15558,27 +15094,15 @@
         <v>0</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>0</v>
@@ -15593,27 +15117,15 @@
         <v>1</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>0</v>
@@ -15628,27 +15140,15 @@
         <v>1</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>0</v>
@@ -15663,27 +15163,15 @@
         <v>1</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>0</v>
@@ -15699,26 +15187,14 @@
       </c>
       <c r="G42" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="H42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>0</v>
@@ -15733,27 +15209,15 @@
         <v>1</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="27" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>0</v>
@@ -15769,26 +15233,14 @@
       </c>
       <c r="G44" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="27" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>0</v>
@@ -15803,27 +15255,15 @@
         <v>0</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K45" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>0</v>
@@ -15839,26 +15279,14 @@
       </c>
       <c r="G46" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="H46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K46" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>0</v>
@@ -15874,26 +15302,14 @@
       </c>
       <c r="G47" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="H47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K47" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>0</v>
@@ -15909,26 +15325,14 @@
       </c>
       <c r="G48" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="H48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K48" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="27" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B49" s="27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>0</v>
@@ -15944,26 +15348,14 @@
       </c>
       <c r="G49" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="H49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J49" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>0</v>
@@ -15979,18 +15371,6 @@
       </c>
       <c r="G50" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="H50" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K50" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>